<commit_message>
Functioning Version used for testing with LCDMPC, before final commenting
</commit_message>
<xml_diff>
--- a/Storage/B_viz_Byzantine.xlsx
+++ b/Storage/B_viz_Byzantine.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spaul/Documents/BlockchainTest/Storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2B2A47-058E-274D-9E7F-78A24A48F005}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973C7ED2-84B6-4942-8A24-3816DE549EBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{802074B0-0BD2-B14A-8923-6BA4D5325CF0}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{802074B0-0BD2-B14A-8923-6BA4D5325CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,7 +180,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -193,7 +193,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400"/>
               <a:t>Byzantine Fault Tolerance Test</a:t>
             </a:r>
           </a:p>
@@ -212,7 +212,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5204,7 +5204,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -5217,7 +5217,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1600"/>
                   <a:t>Block Index</a:t>
                 </a:r>
               </a:p>
@@ -5236,7 +5236,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -5270,11 +5270,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5324,7 +5324,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -5337,7 +5337,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1600"/>
                   <a:t>UtilityToken Balance</a:t>
                 </a:r>
               </a:p>
@@ -5356,7 +5356,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -5388,7 +5388,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6507,7 +6507,7 @@
   <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:AB1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>